<commit_message>
Fixes made to RES, PWR and CCS and reports (pre AFOLU and Waste)
</commit_message>
<xml_diff>
--- a/SATIM/DataSpreadsheets/CO2CAP.xlsx
+++ b/SATIM/DataSpreadsheets/CO2CAP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE\SATIM\DataSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C012E87-DBFD-40E1-A09F-06EE8A2C1572}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3236194-6BE3-4810-9EE9-2DF55031103F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="0" windowWidth="28770" windowHeight="15600" activeTab="5" xr2:uid="{7C70B42E-9201-48A9-B8F0-1466C79FDCED}"/>
+    <workbookView xWindow="1215" yWindow="195" windowWidth="25785" windowHeight="15345" activeTab="2" xr2:uid="{7C70B42E-9201-48A9-B8F0-1466C79FDCED}"/>
   </bookViews>
   <sheets>
     <sheet name="CO2CapInputs" sheetId="5" r:id="rId1"/>
@@ -151,6 +151,24 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={ACCED883-81B4-47FE-8C8B-8B06F399309B}</author>
+  </authors>
+  <commentList>
+    <comment ref="J9" authorId="0" shapeId="0" xr:uid="{ACCED883-81B4-47FE-8C8B-8B06F399309B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Changed to AR5 - August 2021</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author>tc={647BAB51-5A25-4CB6-AABB-CB136337B484}</author>
   </authors>
   <commentList>
@@ -819,6 +837,55 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>48877</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F18C802-5F15-4885-AAA7-DEB8C633E44E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3609975" y="5343525"/>
+          <a:ext cx="6848475" cy="2153902"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -1582,6 +1649,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Bruno Merven" id="{B7CE7B37-9666-44B7-80C8-05E0149DF210}" userId="Bruno Merven" providerId="None"/>
   <person displayName="bruno merven" id="{DADA8B7C-6E4B-4E35-9F47-B4A79E759B90}" userId="144eb91ed0ec6402" providerId="Windows Live"/>
 </personList>
 </file>
@@ -1883,6 +1951,14 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="J9" dT="2021-08-25T15:55:52.62" personId="{B7CE7B37-9666-44B7-80C8-05E0149DF210}" id="{ACCED883-81B4-47FE-8C8B-8B06F399309B}">
+    <text>Changed to AR5 - August 2021</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="J2" dT="2020-10-08T19:45:36.79" personId="{DADA8B7C-6E4B-4E35-9F47-B4A79E759B90}" id="{647BAB51-5A25-4CB6-AABB-CB136337B484}">
     <text>This is a coefficient calculated on the 2017 IPPU CO2eq emissions for the chemicals sector.</text>
   </threadedComment>
@@ -3327,14 +3403,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{987AC606-03E6-4E53-AE7B-7349668CD223}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{987AC606-03E6-4E53-AE7B-7349668CD223}">
   <sheetPr codeName="Sheet4">
     <tabColor theme="4"/>
   </sheetPr>
   <dimension ref="A1:AP27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3718,7 +3794,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.2">
@@ -3747,7 +3823,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.2">
@@ -3776,7 +3852,7 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.2">
@@ -3805,7 +3881,7 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.2">
@@ -3834,7 +3910,7 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.2">
@@ -3863,7 +3939,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:42" x14ac:dyDescent="0.2">
@@ -3892,7 +3968,7 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:42" x14ac:dyDescent="0.2">
@@ -3921,7 +3997,7 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <v>310</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
@@ -3950,7 +4026,7 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>310</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
@@ -3979,7 +4055,7 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>310</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
@@ -4008,7 +4084,7 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>310</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
@@ -4037,7 +4113,7 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>310</v>
+        <v>265</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
@@ -4066,7 +4142,7 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>310</v>
+        <v>265</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
@@ -4095,7 +4171,7 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>310</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
@@ -4153,7 +4229,7 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
@@ -4211,7 +4287,7 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <v>6500</v>
+        <v>6630</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
@@ -4240,11 +4316,13 @@
         <v>0</v>
       </c>
       <c r="J27">
-        <v>9200</v>
+        <v>11000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4610,7 +4688,7 @@
   </sheetPr>
   <dimension ref="A1:AP4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AN4" sqref="AN4:AP4"/>
     </sheetView>
   </sheetViews>

</xml_diff>